<commit_message>
SignIn, Enter, ChangeName 작동 확인
</commit_message>
<xml_diff>
--- a/Data/Excel/Packet/Packet.xlsx
+++ b/Data/Excel/Packet/Packet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SeogyoungWorks\GameServerStudyAspNet\Data\Excel\Packet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitWorks\GameServerStudyAspNet\Data\Excel\Packet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{592DF5DD-83FC-4111-92D8-FD0B65330AB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9AB75C3-CDFD-4B91-B24B-7147D10196F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B14C0FCD-ADAC-43B5-88EF-CD027C78C01B}"/>
+    <workbookView xWindow="13635" yWindow="2205" windowWidth="12750" windowHeight="11295" xr2:uid="{B14C0FCD-ADAC-43B5-88EF-CD027C78C01B}"/>
   </bookViews>
   <sheets>
     <sheet name="Packet" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="39">
   <si>
     <t>ClassInfo</t>
   </si>
@@ -108,7 +108,47 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>title/enter</t>
+    <t>ChannelKey</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ClientSecret</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>AccountEnv</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>AccountState</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>EAccountState</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Result</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SignInResult</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SignInResultPacket</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>common</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>game/enter</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1046,19 +1086,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FCC6768-C9E8-4795-B55A-C1C942DE1B76}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.88671875" customWidth="1"/>
-    <col min="3" max="3" width="16.88671875" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1081,7 +1121,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1089,110 +1129,110 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
       </c>
       <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="E6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="B9" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D10" t="s">
         <v>8</v>
@@ -1201,104 +1241,187 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1" t="s">
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E19" s="1">
         <v>2</v>
       </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1" t="s">
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B15" t="s">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>22</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C21" t="s">
         <v>24</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D21" t="s">
         <v>8</v>
       </c>
-      <c r="E15">
+      <c r="E21">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="1" t="s">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B17" t="s">
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>25</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C23" t="s">
         <v>24</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D23" t="s">
         <v>8</v>
       </c>
-      <c r="E17">
+      <c r="E23">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Construct 로직 작업중 (TODO: ValidEmptyTile)
</commit_message>
<xml_diff>
--- a/Data/Excel/Packet/Packet.xlsx
+++ b/Data/Excel/Packet/Packet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitWorks\GameServerStudyAspNet\Data\Excel\Packet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBA0E954-6200-4A9E-92E1-8E0A496C29A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06B3839-517B-4D77-9A21-872F8786F36B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B14C0FCD-ADAC-43B5-88EF-CD027C78C01B}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="119">
   <si>
     <t>ClassInfo</t>
   </si>
@@ -431,10 +431,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>EndTilePos</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>req</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -468,6 +464,10 @@
   </si>
   <si>
     <t>kingdom/change-item</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>TileSize</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1405,10 +1405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FCC6768-C9E8-4795-B55A-C1C942DE1B76}">
-  <dimension ref="A1:G74"/>
+  <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="D77" sqref="D77"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
@@ -1988,44 +1988,44 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B41" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C41" t="s">
-        <v>109</v>
-      </c>
-      <c r="D41" t="s">
-        <v>107</v>
-      </c>
-      <c r="E41">
-        <v>6</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A42" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="B42" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
+      <c r="C42" t="s">
+        <v>64</v>
+      </c>
+      <c r="D42" t="s">
+        <v>62</v>
+      </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B43" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C43" t="s">
-        <v>64</v>
+        <v>96</v>
       </c>
       <c r="D43" t="s">
-        <v>62</v>
+        <v>95</v>
       </c>
       <c r="E43">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
@@ -2033,42 +2033,42 @@
         <v>72</v>
       </c>
       <c r="C44" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="D44" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="E44">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B45" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C45" t="s">
-        <v>102</v>
-      </c>
-      <c r="D45" t="s">
-        <v>103</v>
-      </c>
-      <c r="E45">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="1" t="s">
-        <v>9</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B46" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1" t="s">
-        <v>79</v>
+      <c r="C46" t="s">
+        <v>41</v>
+      </c>
+      <c r="D46" t="s">
+        <v>40</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.35">
@@ -2076,386 +2076,358 @@
         <v>67</v>
       </c>
       <c r="C47" t="s">
-        <v>41</v>
+        <v>108</v>
       </c>
       <c r="D47" t="s">
-        <v>40</v>
+        <v>107</v>
       </c>
       <c r="E47">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A48" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B48" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C48" t="s">
-        <v>108</v>
-      </c>
-      <c r="D48" t="s">
-        <v>107</v>
-      </c>
-      <c r="E48">
-        <v>3</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B49" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C49" t="s">
-        <v>109</v>
+        <v>65</v>
       </c>
       <c r="D49" t="s">
-        <v>107</v>
+        <v>63</v>
       </c>
       <c r="E49">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A50" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="B50" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C50" t="s">
+        <v>96</v>
+      </c>
+      <c r="D50" t="s">
+        <v>95</v>
+      </c>
+      <c r="E50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B51" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C51" t="s">
-        <v>65</v>
-      </c>
-      <c r="D51" t="s">
-        <v>63</v>
-      </c>
-      <c r="E51">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+        <v>83</v>
+      </c>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="1"/>
       <c r="B52" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C52" t="s">
-        <v>96</v>
+        <v>83</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="D52" t="s">
-        <v>95</v>
-      </c>
-      <c r="E52">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="1" t="s">
-        <v>9</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="E52" s="1">
+        <v>2</v>
+      </c>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B53" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A54" s="1"/>
+      <c r="C53" t="s">
+        <v>91</v>
+      </c>
+      <c r="D53" t="s">
+        <v>77</v>
+      </c>
+      <c r="E53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A54" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B54" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D54" t="s">
-        <v>90</v>
-      </c>
-      <c r="E54" s="1">
-        <v>2</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="C54" s="1"/>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B55" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C55" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="D55" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E55">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A56" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="B56" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
+      <c r="C56" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D56" t="s">
+        <v>75</v>
+      </c>
+      <c r="E56" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B57" s="1" t="s">
         <v>84</v>
       </c>
       <c r="C57" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="D57" t="s">
-        <v>76</v>
-      </c>
-      <c r="E57">
-        <v>2</v>
+        <v>95</v>
+      </c>
+      <c r="E57" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A58" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="B58" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D58" t="s">
-        <v>75</v>
-      </c>
-      <c r="E58" s="1">
-        <v>3</v>
+        <v>85</v>
+      </c>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A59" s="1"/>
       <c r="B59" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C59" t="s">
-        <v>96</v>
-      </c>
-      <c r="D59" t="s">
-        <v>95</v>
+        <v>85</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="E59" s="1">
-        <v>4</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A60" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="B60" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
-      <c r="G60" s="1" t="s">
-        <v>92</v>
+      <c r="C60" t="s">
+        <v>41</v>
+      </c>
+      <c r="D60" t="s">
+        <v>40</v>
+      </c>
+      <c r="E60">
+        <v>3</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A61" s="1"/>
       <c r="B61" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="E61" s="1">
-        <v>2</v>
-      </c>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
+      <c r="C61" t="s">
+        <v>42</v>
+      </c>
+      <c r="D61" t="s">
+        <v>40</v>
+      </c>
+      <c r="E61">
+        <v>4</v>
+      </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B62" s="1" t="s">
         <v>85</v>
       </c>
       <c r="C62" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D62" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="E62">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A63" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B63" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C63" t="s">
-        <v>42</v>
-      </c>
-      <c r="D63" t="s">
-        <v>40</v>
-      </c>
-      <c r="E63">
-        <v>4</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B64" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C64" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="D64" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E64">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A65" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="B65" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
-      <c r="G65" s="1"/>
+      <c r="C65" t="s">
+        <v>48</v>
+      </c>
+      <c r="D65" t="s">
+        <v>51</v>
+      </c>
+      <c r="E65">
+        <v>3</v>
+      </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>109</v>
+      </c>
       <c r="B66" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C66" t="s">
-        <v>64</v>
-      </c>
-      <c r="D66" t="s">
-        <v>61</v>
-      </c>
-      <c r="E66">
-        <v>2</v>
+        <v>112</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B67" s="1" t="s">
-        <v>86</v>
+        <v>112</v>
       </c>
       <c r="C67" t="s">
-        <v>48</v>
+        <v>113</v>
       </c>
       <c r="D67" t="s">
-        <v>51</v>
+        <v>90</v>
       </c>
       <c r="E67">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B68" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C68" t="s">
+        <v>114</v>
+      </c>
+      <c r="D68" t="s">
+        <v>116</v>
+      </c>
+      <c r="E68">
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
-        <v>110</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A69" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="B69" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C69" t="s">
-        <v>114</v>
-      </c>
-      <c r="D69" t="s">
-        <v>90</v>
-      </c>
-      <c r="E69">
-        <v>2</v>
+        <v>111</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B70" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C70" t="s">
-        <v>115</v>
+        <v>96</v>
       </c>
       <c r="D70" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
       <c r="E70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B71" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C71" t="s">
+        <v>74</v>
+      </c>
+      <c r="D71" t="s">
+        <v>76</v>
+      </c>
+      <c r="E71">
         <v>3</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A71" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B72" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C72" t="s">
-        <v>96</v>
+        <v>111</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="D72" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="E72">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B73" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C73" t="s">
-        <v>74</v>
-      </c>
-      <c r="D73" t="s">
-        <v>76</v>
-      </c>
-      <c r="E73">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B74" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D74" t="s">
-        <v>75</v>
-      </c>
-      <c r="E74">
         <v>4</v>
       </c>
     </row>
@@ -2468,10 +2440,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98ECFAC6-7668-4D7C-8368-FE9C0BD686E8}">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.35"/>
@@ -2851,22 +2823,22 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+      <c r="A28" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B28" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C29" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D29" t="s">
-        <v>88</v>
+        <v>40</v>
       </c>
       <c r="E29">
         <v>1</v>
@@ -2874,10 +2846,10 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C30" t="s">
-        <v>56</v>
+        <v>106</v>
       </c>
       <c r="D30" t="s">
         <v>40</v>
@@ -2887,16 +2859,52 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>37</v>
+      </c>
       <c r="B31" t="s">
-        <v>116</v>
-      </c>
-      <c r="C31" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
+        <v>115</v>
+      </c>
+      <c r="C32" t="s">
+        <v>110</v>
+      </c>
+      <c r="D32" t="s">
+        <v>88</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B33" t="s">
+        <v>115</v>
+      </c>
+      <c r="C33" t="s">
+        <v>56</v>
+      </c>
+      <c r="D33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
+        <v>115</v>
+      </c>
+      <c r="C34" t="s">
         <v>104</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D34" t="s">
         <v>107</v>
       </c>
-      <c r="E31">
+      <c r="E34">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
kingdom api 응답값 추가
</commit_message>
<xml_diff>
--- a/Data/Excel/Packet/Packet.xlsx
+++ b/Data/Excel/Packet/Packet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitWorks\GameServerStudyAspNet\Data\Excel\Packet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C039637-E384-45CD-B7F7-0EB23A936998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA53B3A-2E80-46F8-B782-BD1D760182D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6825" yWindow="1830" windowWidth="21600" windowHeight="11295" xr2:uid="{B14C0FCD-ADAC-43B5-88EF-CD027C78C01B}"/>
+    <workbookView xWindow="6825" yWindow="1830" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{B14C0FCD-ADAC-43B5-88EF-CD027C78C01B}"/>
   </bookViews>
   <sheets>
     <sheet name="Packet" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="124">
   <si>
     <t>ClassInfo</t>
   </si>
@@ -182,10 +182,6 @@
   </si>
   <si>
     <t>Amount</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>long</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -1431,8 +1427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FCC6768-C9E8-4795-B55A-C1C942DE1B76}">
   <dimension ref="A1:G83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="G74" sqref="G74"/>
+    <sheetView topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1774,19 +1770,19 @@
         <v>9</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
       <c r="G24" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C25" t="s">
         <v>41</v>
@@ -1800,13 +1796,13 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C26" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" t="s">
         <v>57</v>
-      </c>
-      <c r="D26" t="s">
-        <v>58</v>
       </c>
       <c r="E26">
         <v>3</v>
@@ -1817,7 +1813,7 @@
         <v>13</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -1827,13 +1823,13 @@
     </row>
     <row r="28" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C28" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E28">
         <v>2</v>
@@ -1841,13 +1837,13 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C29" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E29">
         <v>3</v>
@@ -1858,19 +1854,19 @@
         <v>9</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C31" t="s">
         <v>41</v>
@@ -1884,13 +1880,13 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C32" t="s">
+        <v>56</v>
+      </c>
+      <c r="D32" t="s">
         <v>57</v>
-      </c>
-      <c r="D32" t="s">
-        <v>58</v>
       </c>
       <c r="E32">
         <v>3</v>
@@ -1901,7 +1897,7 @@
         <v>13</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -1911,13 +1907,13 @@
     </row>
     <row r="34" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C34" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E34">
         <v>2</v>
@@ -1925,13 +1921,13 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C35" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D35" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E35">
         <v>3</v>
@@ -1942,26 +1938,26 @@
         <v>9</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C37" t="s">
+        <v>85</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="E37">
         <v>2</v>
@@ -1971,7 +1967,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C38" t="s">
         <v>41</v>
@@ -1985,13 +1981,13 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C39" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D39" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E39">
         <v>4</v>
@@ -1999,13 +1995,13 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C40" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D40" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E40">
         <v>5</v>
@@ -2016,7 +2012,7 @@
         <v>13</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
@@ -2026,13 +2022,13 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D42" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E42">
         <v>2</v>
@@ -2040,13 +2036,13 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C43" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D43" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E43">
         <v>3</v>
@@ -2054,13 +2050,13 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C44" t="s">
+        <v>98</v>
+      </c>
+      <c r="D44" t="s">
         <v>99</v>
-      </c>
-      <c r="D44" t="s">
-        <v>100</v>
       </c>
       <c r="E44">
         <v>4</v>
@@ -2071,19 +2067,19 @@
         <v>9</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C46" t="s">
         <v>41</v>
@@ -2097,13 +2093,13 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C47" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D47" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E47">
         <v>3</v>
@@ -2114,7 +2110,7 @@
         <v>13</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
@@ -2124,13 +2120,13 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C49" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D49" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E49">
         <v>2</v>
@@ -2138,13 +2134,13 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C50" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D50" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E50">
         <v>3</v>
@@ -2155,26 +2151,26 @@
         <v>9</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D52" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E52" s="1">
         <v>2</v>
@@ -2187,7 +2183,7 @@
         <v>13</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
@@ -2197,13 +2193,13 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C54" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D54" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E54">
         <v>2</v>
@@ -2211,13 +2207,13 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D55" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E55" s="1">
         <v>3</v>
@@ -2225,13 +2221,13 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C56" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D56" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E56" s="1">
         <v>4</v>
@@ -2242,26 +2238,26 @@
         <v>9</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
       <c r="G57" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C58" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="E58" s="1">
         <v>2</v>
@@ -2271,7 +2267,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C59" t="s">
         <v>41</v>
@@ -2285,7 +2281,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C60" t="s">
         <v>42</v>
@@ -2299,13 +2295,13 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C61" t="s">
         <v>43</v>
       </c>
       <c r="D61" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E61">
         <v>5</v>
@@ -2316,7 +2312,7 @@
         <v>13</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
@@ -2326,13 +2322,13 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B63" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C63" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E63">
         <v>2</v>
@@ -2340,13 +2336,13 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C64" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D64" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E64">
         <v>3</v>
@@ -2354,24 +2350,24 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C66" t="s">
         <v>109</v>
       </c>
-      <c r="C66" t="s">
-        <v>110</v>
-      </c>
       <c r="D66" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E66">
         <v>2</v>
@@ -2379,13 +2375,13 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C67" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D67" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E67">
         <v>3</v>
@@ -2393,13 +2389,13 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C68" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D68" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E68">
         <v>3</v>
@@ -2410,18 +2406,18 @@
         <v>13</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B70" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C70" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D70" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E70">
         <v>2</v>
@@ -2429,13 +2425,13 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B71" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C71" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D71" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E71">
         <v>3</v>
@@ -2443,13 +2439,13 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B72" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D72" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E72">
         <v>4</v>
@@ -2460,26 +2456,26 @@
         <v>9</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
       <c r="G73" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C74" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D74" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="E74" s="1">
         <v>2</v>
@@ -2489,7 +2485,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B75" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C75" t="s">
         <v>41</v>
@@ -2506,7 +2502,7 @@
         <v>13</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
@@ -2516,13 +2512,13 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B77" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C77" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D77" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E77">
         <v>2</v>
@@ -2533,26 +2529,26 @@
         <v>9</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
       <c r="G78" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C79" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D79" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="E79" s="1">
         <v>2</v>
@@ -2562,7 +2558,7 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B80" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C80" t="s">
         <v>41</v>
@@ -2579,7 +2575,7 @@
         <v>13</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
@@ -2589,13 +2585,13 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B82" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C82" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D82" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E82">
         <v>2</v>
@@ -2603,13 +2599,13 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B83" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C83" t="s">
+        <v>98</v>
+      </c>
+      <c r="D83" t="s">
         <v>99</v>
-      </c>
-      <c r="D83" t="s">
-        <v>100</v>
       </c>
       <c r="E83" s="1">
         <v>3</v>
@@ -2626,8 +2622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98ECFAC6-7668-4D7C-8368-FE9C0BD686E8}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2672,7 +2668,7 @@
         <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -2682,13 +2678,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -2696,10 +2692,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D5" t="s">
         <v>40</v>
@@ -2710,13 +2706,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C6" t="s">
         <v>46</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E6">
         <v>3</v>
@@ -2724,13 +2720,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C7" t="s">
         <v>96</v>
       </c>
-      <c r="C7" t="s">
-        <v>97</v>
-      </c>
       <c r="D7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E7">
         <v>4</v>
@@ -2741,7 +2737,7 @@
         <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
@@ -2751,13 +2747,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" t="s">
         <v>54</v>
       </c>
-      <c r="C9" t="s">
-        <v>55</v>
-      </c>
       <c r="D9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -2765,10 +2761,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D10" t="s">
         <v>40</v>
@@ -2779,13 +2775,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
         <v>46</v>
       </c>
       <c r="D11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E11">
         <v>3</v>
@@ -2796,7 +2792,7 @@
         <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -2806,13 +2802,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -2820,10 +2816,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D14" t="s">
         <v>40</v>
@@ -2834,13 +2830,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C15" t="s">
         <v>46</v>
       </c>
       <c r="D15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E15">
         <v>3</v>
@@ -2848,13 +2844,13 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C16" t="s">
         <v>44</v>
       </c>
       <c r="D16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E16">
         <v>3</v>
@@ -2862,13 +2858,13 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C17" t="s">
         <v>45</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E17">
         <v>3</v>
@@ -2879,7 +2875,7 @@
         <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
@@ -2889,13 +2885,13 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C19" t="s">
         <v>44</v>
       </c>
       <c r="D19" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -2903,13 +2899,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C20" t="s">
         <v>45</v>
       </c>
       <c r="D20" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E20">
         <v>2</v>
@@ -2917,13 +2913,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C21" t="s">
         <v>46</v>
       </c>
       <c r="D21" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E21">
         <v>3</v>
@@ -2934,7 +2930,7 @@
         <v>37</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
@@ -2944,13 +2940,13 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" t="s">
         <v>48</v>
       </c>
-      <c r="C23" t="s">
-        <v>49</v>
-      </c>
       <c r="D23" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E23">
         <v>1</v>
@@ -2958,13 +2954,13 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D24" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E24">
         <v>2</v>
@@ -2975,15 +2971,15 @@
         <v>37</v>
       </c>
       <c r="B25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" t="s">
         <v>101</v>
-      </c>
-      <c r="C26" t="s">
-        <v>102</v>
       </c>
       <c r="D26" t="s">
         <v>40</v>
@@ -2994,10 +2990,10 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D27" t="s">
         <v>40</v>
@@ -3011,15 +3007,15 @@
         <v>37</v>
       </c>
       <c r="B28" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D29" t="s">
         <v>40</v>
@@ -3030,10 +3026,10 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D30" t="s">
         <v>40</v>
@@ -3047,18 +3043,18 @@
         <v>37</v>
       </c>
       <c r="B31" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C32" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -3066,13 +3062,13 @@
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E33">
         <v>2</v>
@@ -3080,10 +3076,10 @@
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C34" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D34" t="s">
         <v>40</v>
@@ -3094,13 +3090,13 @@
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C35" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D35" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E35">
         <v>4</v>

</xml_diff>

<commit_message>
Client 에서 Cookie Enhance 호출
</commit_message>
<xml_diff>
--- a/Data/Excel/Packet/Packet.xlsx
+++ b/Data/Excel/Packet/Packet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitWorks\GameServerStudyAspNet\Data\Excel\Packet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADCD1F29-0FB5-45C2-AD52-F3D44985FEC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10F7002-79FC-4E07-94DD-06D97E0B14C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="3435" windowWidth="22980" windowHeight="11295" xr2:uid="{B14C0FCD-ADAC-43B5-88EF-CD027C78C01B}"/>
+    <workbookView xWindow="2025" yWindow="3780" windowWidth="22980" windowHeight="11295" xr2:uid="{B14C0FCD-ADAC-43B5-88EF-CD027C78C01B}"/>
   </bookViews>
   <sheets>
     <sheet name="Packet" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="161">
   <si>
     <t>ClassInfo</t>
   </si>
@@ -636,14 +636,6 @@
   </si>
   <si>
     <t>UsedSoulStone</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>BefAccSoulStone</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>AftAccSoulStone</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1584,10 +1576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FCC6768-C9E8-4795-B55A-C1C942DE1B76}">
-  <dimension ref="A1:G120"/>
+  <dimension ref="A1:G118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
-      <selection activeCell="C101" sqref="C101"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2853,73 +2845,73 @@
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B91" t="s">
-        <v>132</v>
-      </c>
-      <c r="C91" t="s">
-        <v>161</v>
-      </c>
-      <c r="D91" t="s">
-        <v>40</v>
-      </c>
-      <c r="E91">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C91" s="1"/>
+      <c r="D91" s="1"/>
+      <c r="E91" s="1"/>
+      <c r="F91" s="1"/>
+      <c r="G91" s="1"/>
+    </row>
+    <row r="92" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C92" t="s">
-        <v>162</v>
+        <v>134</v>
       </c>
       <c r="D92" t="s">
-        <v>40</v>
+        <v>135</v>
       </c>
       <c r="E92">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
-      <c r="G93" s="1"/>
-    </row>
-    <row r="94" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G93" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="C94" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="D94" t="s">
-        <v>135</v>
+        <v>40</v>
       </c>
       <c r="E94">
         <v>2</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B95" s="1" t="s">
+      <c r="B95" t="s">
         <v>138</v>
       </c>
-      <c r="C95" s="1"/>
-      <c r="D95" s="1"/>
-      <c r="E95" s="1"/>
-      <c r="F95" s="1"/>
-      <c r="G95" s="1" t="s">
-        <v>137</v>
+      <c r="C95" t="s">
+        <v>143</v>
+      </c>
+      <c r="D95" t="s">
+        <v>40</v>
+      </c>
+      <c r="E95">
+        <v>3</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -2927,13 +2919,13 @@
         <v>138</v>
       </c>
       <c r="C96" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D96" t="s">
         <v>40</v>
       </c>
       <c r="E96">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -2941,103 +2933,103 @@
         <v>138</v>
       </c>
       <c r="C97" t="s">
-        <v>143</v>
+        <v>56</v>
       </c>
       <c r="D97" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="E97">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>13</v>
+      </c>
       <c r="B98" t="s">
-        <v>138</v>
-      </c>
-      <c r="C98" t="s">
-        <v>144</v>
-      </c>
-      <c r="D98" t="s">
-        <v>40</v>
-      </c>
-      <c r="E98">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C99" t="s">
-        <v>56</v>
+        <v>134</v>
       </c>
       <c r="D99" t="s">
-        <v>57</v>
+        <v>135</v>
       </c>
       <c r="E99">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>13</v>
-      </c>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B101" t="s">
-        <v>139</v>
-      </c>
-      <c r="C101" t="s">
-        <v>134</v>
-      </c>
-      <c r="D101" t="s">
-        <v>135</v>
-      </c>
-      <c r="E101">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B102" t="s">
-        <v>139</v>
-      </c>
-      <c r="C102" t="s">
+      <c r="C100" t="s">
         <v>95</v>
       </c>
-      <c r="D102" t="s">
+      <c r="D100" t="s">
         <v>97</v>
       </c>
-      <c r="E102">
+      <c r="E100">
         <v>3</v>
       </c>
     </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B101" s="2"/>
+      <c r="C101" s="2"/>
+      <c r="D101" s="2"/>
+      <c r="E101" s="2"/>
+      <c r="F101" s="2"/>
+      <c r="G101" s="2"/>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C102" s="1"/>
+      <c r="D102" s="1"/>
+      <c r="E102" s="1"/>
+      <c r="F102" s="1"/>
+      <c r="G102" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="B103" s="2"/>
-      <c r="C103" s="2"/>
-      <c r="D103" s="2"/>
-      <c r="E103" s="2"/>
-      <c r="F103" s="2"/>
-      <c r="G103" s="2"/>
+      <c r="B103" t="s">
+        <v>145</v>
+      </c>
+      <c r="C103" t="s">
+        <v>147</v>
+      </c>
+      <c r="D103" t="s">
+        <v>40</v>
+      </c>
+      <c r="E103">
+        <v>2</v>
+      </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B104" s="1" t="s">
+      <c r="B104" t="s">
         <v>145</v>
       </c>
-      <c r="C104" s="1"/>
-      <c r="D104" s="1"/>
-      <c r="E104" s="1"/>
-      <c r="F104" s="1"/>
-      <c r="G104" s="1" t="s">
-        <v>159</v>
+      <c r="C104" t="s">
+        <v>148</v>
+      </c>
+      <c r="D104" t="s">
+        <v>40</v>
+      </c>
+      <c r="E104">
+        <v>3</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -3045,215 +3037,187 @@
         <v>145</v>
       </c>
       <c r="C105" t="s">
-        <v>147</v>
+        <v>56</v>
       </c>
       <c r="D105" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="E105">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B106" t="s">
-        <v>145</v>
-      </c>
-      <c r="C106" t="s">
-        <v>148</v>
-      </c>
-      <c r="D106" t="s">
-        <v>40</v>
-      </c>
-      <c r="E106">
-        <v>3</v>
-      </c>
+      <c r="A106" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C106" s="1"/>
+      <c r="D106" s="1"/>
+      <c r="E106" s="1"/>
+      <c r="F106" s="1"/>
+      <c r="G106" s="1"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C107" t="s">
-        <v>56</v>
+        <v>149</v>
       </c>
       <c r="D107" t="s">
-        <v>57</v>
+        <v>99</v>
       </c>
       <c r="E107">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B108" s="1" t="s">
+      <c r="B108" t="s">
         <v>146</v>
       </c>
-      <c r="C108" s="1"/>
-      <c r="D108" s="1"/>
-      <c r="E108" s="1"/>
-      <c r="F108" s="1"/>
-      <c r="G108" s="1"/>
+      <c r="C108" t="s">
+        <v>150</v>
+      </c>
+      <c r="D108" t="s">
+        <v>97</v>
+      </c>
+      <c r="E108">
+        <v>3</v>
+      </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B109" t="s">
-        <v>146</v>
-      </c>
-      <c r="C109" t="s">
-        <v>149</v>
-      </c>
-      <c r="D109" t="s">
-        <v>99</v>
-      </c>
-      <c r="E109">
-        <v>2</v>
-      </c>
+      <c r="A109" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B109" s="2"/>
+      <c r="C109" s="2"/>
+      <c r="D109" s="2"/>
+      <c r="E109" s="2"/>
+      <c r="F109" s="2"/>
+      <c r="G109" s="2"/>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B110" t="s">
-        <v>146</v>
-      </c>
-      <c r="C110" t="s">
-        <v>150</v>
-      </c>
-      <c r="D110" t="s">
-        <v>97</v>
-      </c>
-      <c r="E110">
-        <v>3</v>
+      <c r="A110" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C110" s="1"/>
+      <c r="D110" s="1"/>
+      <c r="E110" s="1"/>
+      <c r="F110" s="1"/>
+      <c r="G110" s="1" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B111" s="2"/>
-      <c r="C111" s="2"/>
-      <c r="D111" s="2"/>
-      <c r="E111" s="2"/>
-      <c r="F111" s="2"/>
-      <c r="G111" s="2"/>
+      <c r="B111" t="s">
+        <v>126</v>
+      </c>
+      <c r="C111" t="s">
+        <v>128</v>
+      </c>
+      <c r="D111" t="s">
+        <v>129</v>
+      </c>
+      <c r="E111">
+        <v>2</v>
+      </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
-      <c r="G112" s="1" t="s">
-        <v>130</v>
-      </c>
+      <c r="G112" s="1"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C113" t="s">
-        <v>128</v>
+        <v>98</v>
       </c>
       <c r="D113" t="s">
-        <v>129</v>
+        <v>99</v>
       </c>
       <c r="E113">
         <v>2</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C114" s="1"/>
-      <c r="D114" s="1"/>
-      <c r="E114" s="1"/>
-      <c r="F114" s="1"/>
-      <c r="G114" s="1"/>
+      <c r="A114" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B114" s="2"/>
+      <c r="C114" s="2"/>
+      <c r="D114" s="2"/>
+      <c r="E114" s="2"/>
+      <c r="F114" s="2"/>
+      <c r="G114" s="2"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B115" t="s">
-        <v>127</v>
-      </c>
-      <c r="C115" t="s">
-        <v>98</v>
-      </c>
-      <c r="D115" t="s">
-        <v>99</v>
-      </c>
-      <c r="E115">
-        <v>2</v>
+      <c r="A115" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C115" s="1"/>
+      <c r="D115" s="1"/>
+      <c r="E115" s="1"/>
+      <c r="F115" s="1"/>
+      <c r="G115" s="1" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A116" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B116" s="2"/>
-      <c r="C116" s="2"/>
-      <c r="D116" s="2"/>
-      <c r="E116" s="2"/>
-      <c r="F116" s="2"/>
-      <c r="G116" s="2"/>
+      <c r="B116" t="s">
+        <v>152</v>
+      </c>
+      <c r="C116" t="s">
+        <v>156</v>
+      </c>
+      <c r="D116" t="s">
+        <v>157</v>
+      </c>
+      <c r="E116">
+        <v>2</v>
+      </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
       <c r="E117" s="1"/>
       <c r="F117" s="1"/>
-      <c r="G117" s="1" t="s">
-        <v>158</v>
-      </c>
+      <c r="G117" s="1"/>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C118" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D118" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E118">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B119" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C119" s="1"/>
-      <c r="D119" s="1"/>
-      <c r="E119" s="1"/>
-      <c r="F119" s="1"/>
-      <c r="G119" s="1"/>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B120" t="s">
-        <v>153</v>
-      </c>
-      <c r="C120" t="s">
-        <v>154</v>
-      </c>
-      <c r="D120" t="s">
-        <v>155</v>
-      </c>
-      <c r="E120">
         <v>2</v>
       </c>
     </row>

</xml_diff>